<commit_message>
rebuilding site Mo 10. Feb 14:26:15 CET 2020
</commit_message>
<xml_diff>
--- a/schule/excel-zeugnislisten/Dateien/Zeugnisnotenberechnung_Oberstufe_Template.xlsx
+++ b/schule/excel-zeugnislisten/Dateien/Zeugnisnotenberechnung_Oberstufe_Template.xlsx
@@ -143,10 +143,10 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0"/>
     <numFmt numFmtId="167" formatCode="General"/>
-    <numFmt numFmtId="168" formatCode="&quot;LO&quot;G\IS\CH"/>
-    <numFmt numFmtId="169" formatCode="DD/MM/YY"/>
-    <numFmt numFmtId="170" formatCode="DDDD"/>
-    <numFmt numFmtId="171" formatCode="DDDD&quot;, &quot;"/>
+    <numFmt numFmtId="168" formatCode="&quot;LO&quot;g\Is\Ch"/>
+    <numFmt numFmtId="169" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="170" formatCode="dddd"/>
+    <numFmt numFmtId="171" formatCode="dddd&quot;, &quot;"/>
   </numFmts>
   <fonts count="16">
     <font>
@@ -860,12 +860,13 @@
   </sheetPr>
   <dimension ref="A1:BN182"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AI5" activeCellId="0" sqref="AI5:AI6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H45" activeCellId="0" sqref="H45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="4.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.67"/>
@@ -882,9 +883,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="3.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="6.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="4.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="7.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="7.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="4.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="7.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="7.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="4.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="6.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="4.44"/>
@@ -5395,10 +5396,7 @@
         <v>3</v>
       </c>
       <c r="G36" s="45"/>
-      <c r="H36" s="45" t="e">
-        <f aca="false">AVERAGE(H5:H34)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H36" s="45"/>
       <c r="I36" s="45" t="e">
         <f aca="false">AVERAGE(I5:I34)</f>
         <v>#DIV/0!</v>
@@ -5628,7 +5626,7 @@
       <c r="BM37" s="3"/>
       <c r="BN37" s="3"/>
     </row>
-    <row r="38" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3"/>
       <c r="B38" s="46" t="s">
         <v>29</v>
@@ -5646,10 +5644,7 @@
         <v>0</v>
       </c>
       <c r="G38" s="48"/>
-      <c r="H38" s="48" t="n">
-        <f aca="false">COUNTIF(H$5:H$34,"1")</f>
-        <v>0</v>
-      </c>
+      <c r="H38" s="48"/>
       <c r="I38" s="48" t="n">
         <f aca="false">COUNTIF(I$5:I$34,"1")</f>
         <v>0</v>
@@ -5811,7 +5806,7 @@
       <c r="BM38" s="3"/>
       <c r="BN38" s="3"/>
     </row>
-    <row r="39" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3"/>
       <c r="B39" s="49" t="s">
         <v>29</v>
@@ -5829,10 +5824,7 @@
         <v>0</v>
       </c>
       <c r="G39" s="48"/>
-      <c r="H39" s="48" t="n">
-        <f aca="false">COUNTIF(H$5:H$34,"2")</f>
-        <v>1</v>
-      </c>
+      <c r="H39" s="48"/>
       <c r="I39" s="48" t="n">
         <f aca="false">COUNTIF(I$5:I$34,"2")</f>
         <v>1</v>
@@ -5994,7 +5986,7 @@
       <c r="BM39" s="3"/>
       <c r="BN39" s="3"/>
     </row>
-    <row r="40" customFormat="false" ht="25.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3"/>
       <c r="B40" s="49" t="s">
         <v>29</v>
@@ -6012,10 +6004,7 @@
         <v>2</v>
       </c>
       <c r="G40" s="48"/>
-      <c r="H40" s="48" t="n">
-        <f aca="false">COUNTIF(H$5:H$34,"3")</f>
-        <v>0</v>
-      </c>
+      <c r="H40" s="48"/>
       <c r="I40" s="48" t="n">
         <f aca="false">COUNTIF(I$5:I$34,"3")</f>
         <v>1</v>
@@ -6177,7 +6166,7 @@
       <c r="BM40" s="3"/>
       <c r="BN40" s="3"/>
     </row>
-    <row r="41" customFormat="false" ht="25.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3"/>
       <c r="B41" s="49" t="s">
         <v>29</v>
@@ -6195,10 +6184,7 @@
         <v>0</v>
       </c>
       <c r="G41" s="48"/>
-      <c r="H41" s="48" t="n">
-        <f aca="false">COUNTIF(H$5:H$34,"4")</f>
-        <v>0</v>
-      </c>
+      <c r="H41" s="48"/>
       <c r="I41" s="48" t="n">
         <f aca="false">COUNTIF(I$5:I$34,"4")</f>
         <v>0</v>
@@ -6360,7 +6346,7 @@
       <c r="BM41" s="3"/>
       <c r="BN41" s="3"/>
     </row>
-    <row r="42" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3"/>
       <c r="B42" s="49" t="s">
         <v>29</v>
@@ -6378,10 +6364,7 @@
         <v>0</v>
       </c>
       <c r="G42" s="48"/>
-      <c r="H42" s="48" t="n">
-        <f aca="false">COUNTIF(H$5:H$34,"5")</f>
-        <v>0</v>
-      </c>
+      <c r="H42" s="48"/>
       <c r="I42" s="48" t="n">
         <f aca="false">COUNTIF(I$5:I$34,"5")</f>
         <v>0</v>
@@ -6543,7 +6526,7 @@
       <c r="BM42" s="3"/>
       <c r="BN42" s="3"/>
     </row>
-    <row r="43" customFormat="false" ht="25.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3"/>
       <c r="B43" s="51" t="s">
         <v>29</v>
@@ -6561,10 +6544,7 @@
         <v>0</v>
       </c>
       <c r="G43" s="48"/>
-      <c r="H43" s="48" t="n">
-        <f aca="false">COUNTIF(H$5:H$34,"6")</f>
-        <v>0</v>
-      </c>
+      <c r="H43" s="48"/>
       <c r="I43" s="48" t="n">
         <f aca="false">COUNTIF(I$5:I$34,"6")</f>
         <v>0</v>

</xml_diff>